<commit_message>
Merge with upstream (1.8)
</commit_message>
<xml_diff>
--- a/openpyxl/tests/test_data/reader/complex-styles.xlsx
+++ b/openpyxl/tests/test_data/reader/complex-styles.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="17820" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="21">
   <si>
     <t>Arial Font, Italic 14</t>
   </si>
@@ -251,7 +251,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -261,8 +261,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -302,6 +304,9 @@
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -315,15 +320,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -653,152 +660,398 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="31.1640625" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" customWidth="1"/>
+    <col min="5" max="5" width="31.1640625" customWidth="1"/>
+    <col min="7" max="7" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" ht="17">
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="C4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="C5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="C6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="C7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="C8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="C9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="C10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="C11" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="C12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="C13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="C14" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="14">
         <v>1.1234500000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="C15" s="14">
+        <v>1.1234500000000001</v>
+      </c>
+      <c r="E15" s="14">
+        <v>1.1234500000000001</v>
+      </c>
+      <c r="G15" s="14">
+        <v>1.1234500000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="15">
         <v>40939</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" s="15">
+        <v>40939</v>
+      </c>
+      <c r="E16" s="15">
+        <v>40939</v>
+      </c>
+      <c r="G16" s="15">
+        <v>40939</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="16">
         <v>0.1234</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="17" t="s">
+      <c r="C17" s="16">
+        <v>0.1234</v>
+      </c>
+      <c r="E17" s="16">
+        <v>0.1234</v>
+      </c>
+      <c r="G17" s="16">
+        <v>0.1234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="17"/>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="B18" s="23"/>
+      <c r="C18" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="23"/>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="18" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="16" thickBot="1">
+      <c r="C19" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="16" thickBot="1">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="17" thickTop="1" thickBot="1">
       <c r="A21" s="19" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="C21" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="17" thickTop="1" thickBot="1">
       <c r="A22" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="23" t="s">
+      <c r="C22" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="24"/>
-    </row>
-    <row r="24" spans="1:2" ht="16" thickBot="1">
-      <c r="A24" s="25"/>
-      <c r="B24" s="26"/>
-    </row>
-    <row r="25" spans="1:2" ht="30">
+      <c r="B23" s="25"/>
+      <c r="C23" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="25"/>
+      <c r="E23" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="25"/>
+      <c r="G23" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="25"/>
+    </row>
+    <row r="24" spans="1:8" ht="16" thickBot="1">
+      <c r="A24" s="26"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="27"/>
+    </row>
+    <row r="25" spans="1:8" ht="30">
       <c r="A25" s="20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="21" t="s">
         <v>18</v>
       </c>
+      <c r="C26" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="8">
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G23:H24"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A23:B24"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E23:F24"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Merge with Schema Validation.
</commit_message>
<xml_diff>
--- a/openpyxl/tests/test_data/reader/complex-styles.xlsx
+++ b/openpyxl/tests/test_data/reader/complex-styles.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="17820" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="21">
   <si>
     <t>Arial Font, Italic 14</t>
   </si>
@@ -251,7 +251,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -261,8 +261,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -302,6 +304,9 @@
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -315,15 +320,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -653,152 +660,398 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="31.1640625" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" customWidth="1"/>
+    <col min="5" max="5" width="31.1640625" customWidth="1"/>
+    <col min="7" max="7" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" ht="17">
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="C4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="C5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="C6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="C7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="C8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="C9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="C10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="C11" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="C12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="C13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="C14" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="14">
         <v>1.1234500000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="C15" s="14">
+        <v>1.1234500000000001</v>
+      </c>
+      <c r="E15" s="14">
+        <v>1.1234500000000001</v>
+      </c>
+      <c r="G15" s="14">
+        <v>1.1234500000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="15">
         <v>40939</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" s="15">
+        <v>40939</v>
+      </c>
+      <c r="E16" s="15">
+        <v>40939</v>
+      </c>
+      <c r="G16" s="15">
+        <v>40939</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="16">
         <v>0.1234</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="17" t="s">
+      <c r="C17" s="16">
+        <v>0.1234</v>
+      </c>
+      <c r="E17" s="16">
+        <v>0.1234</v>
+      </c>
+      <c r="G17" s="16">
+        <v>0.1234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="17"/>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="B18" s="23"/>
+      <c r="C18" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="23"/>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="18" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="16" thickBot="1">
+      <c r="C19" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="16" thickBot="1">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="17" thickTop="1" thickBot="1">
       <c r="A21" s="19" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="C21" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="17" thickTop="1" thickBot="1">
       <c r="A22" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="23" t="s">
+      <c r="C22" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="24"/>
-    </row>
-    <row r="24" spans="1:2" ht="16" thickBot="1">
-      <c r="A24" s="25"/>
-      <c r="B24" s="26"/>
-    </row>
-    <row r="25" spans="1:2" ht="30">
+      <c r="B23" s="25"/>
+      <c r="C23" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="25"/>
+      <c r="E23" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="25"/>
+      <c r="G23" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="25"/>
+    </row>
+    <row r="24" spans="1:8" ht="16" thickBot="1">
+      <c r="A24" s="26"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="27"/>
+    </row>
+    <row r="25" spans="1:8" ht="30">
       <c r="A25" s="20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="21" t="s">
         <v>18</v>
       </c>
+      <c r="C26" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="8">
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G23:H24"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A23:B24"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E23:F24"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>